<commit_message>
adjusting documentation - running with trimmed categories
</commit_message>
<xml_diff>
--- a/6 glm models/2 historical performance/evaluation_Data.xlsx
+++ b/6 glm models/2 historical performance/evaluation_Data.xlsx
@@ -3297,7 +3297,7 @@
         <v>0.25</v>
       </c>
       <c r="F122" t="n">
-        <v>7401.0</v>
+        <v>7400.0</v>
       </c>
       <c r="G122" t="n">
         <v>0.0</v>
@@ -3323,7 +3323,7 @@
         <v>0.5</v>
       </c>
       <c r="F123" t="n">
-        <v>7401.0</v>
+        <v>7400.0</v>
       </c>
       <c r="G123" t="n">
         <v>0.0</v>
@@ -3349,7 +3349,7 @@
         <v>1.0</v>
       </c>
       <c r="F124" t="n">
-        <v>7401.0</v>
+        <v>7400.0</v>
       </c>
       <c r="G124" t="n">
         <v>0.0</v>
@@ -3375,7 +3375,7 @@
         <v>0.25</v>
       </c>
       <c r="F125" t="n">
-        <v>7401.0</v>
+        <v>7400.0</v>
       </c>
       <c r="G125" t="n">
         <v>0.0</v>
@@ -3401,7 +3401,7 @@
         <v>0.5</v>
       </c>
       <c r="F126" t="n">
-        <v>7401.0</v>
+        <v>7400.0</v>
       </c>
       <c r="G126" t="n">
         <v>0.0</v>
@@ -3427,7 +3427,7 @@
         <v>1.0</v>
       </c>
       <c r="F127" t="n">
-        <v>7401.0</v>
+        <v>7400.0</v>
       </c>
       <c r="G127" t="n">
         <v>0.0</v>
@@ -3453,7 +3453,7 @@
         <v>0.25</v>
       </c>
       <c r="F128" t="n">
-        <v>7401.0</v>
+        <v>7400.0</v>
       </c>
       <c r="G128" t="n">
         <v>0.0</v>
@@ -3479,7 +3479,7 @@
         <v>0.5</v>
       </c>
       <c r="F129" t="n">
-        <v>7401.0</v>
+        <v>7400.0</v>
       </c>
       <c r="G129" t="n">
         <v>0.0</v>
@@ -3505,7 +3505,7 @@
         <v>1.0</v>
       </c>
       <c r="F130" t="n">
-        <v>7401.0</v>
+        <v>7400.0</v>
       </c>
       <c r="G130" t="n">
         <v>0.0</v>
@@ -3531,7 +3531,7 @@
         <v>0.25</v>
       </c>
       <c r="F131" t="n">
-        <v>7401.0</v>
+        <v>7400.0</v>
       </c>
       <c r="G131" t="n">
         <v>0.0</v>
@@ -3557,7 +3557,7 @@
         <v>0.5</v>
       </c>
       <c r="F132" t="n">
-        <v>7401.0</v>
+        <v>7400.0</v>
       </c>
       <c r="G132" t="n">
         <v>0.0</v>
@@ -3583,7 +3583,7 @@
         <v>1.0</v>
       </c>
       <c r="F133" t="n">
-        <v>7401.0</v>
+        <v>7400.0</v>
       </c>
       <c r="G133" t="n">
         <v>0.0</v>
@@ -3609,7 +3609,7 @@
         <v>0.25</v>
       </c>
       <c r="F134" t="n">
-        <v>7401.0</v>
+        <v>7400.0</v>
       </c>
       <c r="G134" t="n">
         <v>0.0</v>
@@ -3635,7 +3635,7 @@
         <v>0.5</v>
       </c>
       <c r="F135" t="n">
-        <v>7401.0</v>
+        <v>7400.0</v>
       </c>
       <c r="G135" t="n">
         <v>0.0</v>
@@ -3661,7 +3661,7 @@
         <v>1.0</v>
       </c>
       <c r="F136" t="n">
-        <v>7401.0</v>
+        <v>7400.0</v>
       </c>
       <c r="G136" t="n">
         <v>0.0</v>
@@ -3687,7 +3687,7 @@
         <v>0.25</v>
       </c>
       <c r="F137" t="n">
-        <v>7401.0</v>
+        <v>7400.0</v>
       </c>
       <c r="G137" t="n">
         <v>0.0</v>
@@ -3713,7 +3713,7 @@
         <v>0.5</v>
       </c>
       <c r="F138" t="n">
-        <v>7401.0</v>
+        <v>7400.0</v>
       </c>
       <c r="G138" t="n">
         <v>0.0</v>
@@ -3739,7 +3739,7 @@
         <v>1.0</v>
       </c>
       <c r="F139" t="n">
-        <v>7401.0</v>
+        <v>7400.0</v>
       </c>
       <c r="G139" t="n">
         <v>0.0</v>
@@ -3765,7 +3765,7 @@
         <v>0.25</v>
       </c>
       <c r="F140" t="n">
-        <v>7401.0</v>
+        <v>7400.0</v>
       </c>
       <c r="G140" t="n">
         <v>0.0</v>
@@ -3791,7 +3791,7 @@
         <v>0.5</v>
       </c>
       <c r="F141" t="n">
-        <v>7401.0</v>
+        <v>7400.0</v>
       </c>
       <c r="G141" t="n">
         <v>0.0</v>
@@ -3817,7 +3817,7 @@
         <v>1.0</v>
       </c>
       <c r="F142" t="n">
-        <v>7401.0</v>
+        <v>7400.0</v>
       </c>
       <c r="G142" t="n">
         <v>0.0</v>
@@ -3843,7 +3843,7 @@
         <v>0.25</v>
       </c>
       <c r="F143" t="n">
-        <v>7401.0</v>
+        <v>7400.0</v>
       </c>
       <c r="G143" t="n">
         <v>0.0</v>
@@ -3869,7 +3869,7 @@
         <v>0.5</v>
       </c>
       <c r="F144" t="n">
-        <v>7401.0</v>
+        <v>7400.0</v>
       </c>
       <c r="G144" t="n">
         <v>0.0</v>
@@ -3895,7 +3895,7 @@
         <v>1.0</v>
       </c>
       <c r="F145" t="n">
-        <v>7401.0</v>
+        <v>7400.0</v>
       </c>
       <c r="G145" t="n">
         <v>0.0</v>
@@ -6420,10 +6420,10 @@
         <v>5894.0</v>
       </c>
       <c r="G242" t="n">
-        <v>3345.0</v>
+        <v>3519.0</v>
       </c>
       <c r="H242" t="n">
-        <v>0.011187850943721487</v>
+        <v>0.00827862729496309</v>
       </c>
     </row>
     <row r="243">
@@ -6446,10 +6446,10 @@
         <v>5894.0</v>
       </c>
       <c r="G243" t="n">
-        <v>3345.0</v>
+        <v>3519.0</v>
       </c>
       <c r="H243" t="n">
-        <v>0.022375701887442975</v>
+        <v>0.01655725458992618</v>
       </c>
     </row>
     <row r="244">
@@ -6472,10 +6472,10 @@
         <v>5894.0</v>
       </c>
       <c r="G244" t="n">
-        <v>3345.0</v>
+        <v>3519.0</v>
       </c>
       <c r="H244" t="n">
-        <v>0.04475140377488595</v>
+        <v>0.03311450917985236</v>
       </c>
     </row>
     <row r="245">
@@ -6498,10 +6498,10 @@
         <v>5894.0</v>
       </c>
       <c r="G245" t="n">
-        <v>2202.0</v>
+        <v>2362.0</v>
       </c>
       <c r="H245" t="n">
-        <v>0.01965613476257367</v>
+        <v>0.015267799358693662</v>
       </c>
     </row>
     <row r="246">
@@ -6524,10 +6524,10 @@
         <v>5894.0</v>
       </c>
       <c r="G246" t="n">
-        <v>2202.0</v>
+        <v>2362.0</v>
       </c>
       <c r="H246" t="n">
-        <v>0.03931226952514734</v>
+        <v>0.030535598717387324</v>
       </c>
     </row>
     <row r="247">
@@ -6550,10 +6550,10 @@
         <v>5894.0</v>
       </c>
       <c r="G247" t="n">
-        <v>2202.0</v>
+        <v>2362.0</v>
       </c>
       <c r="H247" t="n">
-        <v>0.07862453905029468</v>
+        <v>0.06107119743477465</v>
       </c>
     </row>
     <row r="248">
@@ -6576,10 +6576,10 @@
         <v>5894.0</v>
       </c>
       <c r="G248" t="n">
-        <v>1337.0</v>
+        <v>1498.0</v>
       </c>
       <c r="H248" t="n">
-        <v>0.038020355147212914</v>
+        <v>0.02937290595067568</v>
       </c>
     </row>
     <row r="249">
@@ -6602,10 +6602,10 @@
         <v>5894.0</v>
       </c>
       <c r="G249" t="n">
-        <v>1337.0</v>
+        <v>1498.0</v>
       </c>
       <c r="H249" t="n">
-        <v>0.07604071029442583</v>
+        <v>0.05874581190135136</v>
       </c>
     </row>
     <row r="250">
@@ -6628,10 +6628,10 @@
         <v>5894.0</v>
       </c>
       <c r="G250" t="n">
-        <v>1337.0</v>
+        <v>1498.0</v>
       </c>
       <c r="H250" t="n">
-        <v>0.15208142058885166</v>
+        <v>0.11749162380270271</v>
       </c>
     </row>
     <row r="251">
@@ -6654,10 +6654,10 @@
         <v>5894.0</v>
       </c>
       <c r="G251" t="n">
-        <v>780.0</v>
+        <v>928.0</v>
       </c>
       <c r="H251" t="n">
-        <v>0.0707405438334048</v>
+        <v>0.056125233303089724</v>
       </c>
     </row>
     <row r="252">
@@ -6680,10 +6680,10 @@
         <v>5894.0</v>
       </c>
       <c r="G252" t="n">
-        <v>780.0</v>
+        <v>928.0</v>
       </c>
       <c r="H252" t="n">
-        <v>0.1414810876668096</v>
+        <v>0.11225046660617945</v>
       </c>
     </row>
     <row r="253">
@@ -6706,10 +6706,10 @@
         <v>5894.0</v>
       </c>
       <c r="G253" t="n">
-        <v>780.0</v>
+        <v>928.0</v>
       </c>
       <c r="H253" t="n">
-        <v>0.2829621753336192</v>
+        <v>0.2245009332123589</v>
       </c>
     </row>
     <row r="254">
@@ -6732,10 +6732,10 @@
         <v>5894.0</v>
       </c>
       <c r="G254" t="n">
-        <v>3362.0</v>
+        <v>3517.0</v>
       </c>
       <c r="H254" t="n">
-        <v>0.011311197970881445</v>
+        <v>0.008142532211238385</v>
       </c>
     </row>
     <row r="255">
@@ -6758,10 +6758,10 @@
         <v>5894.0</v>
       </c>
       <c r="G255" t="n">
-        <v>3362.0</v>
+        <v>3517.0</v>
       </c>
       <c r="H255" t="n">
-        <v>0.02262239594176289</v>
+        <v>0.01628506442247677</v>
       </c>
     </row>
     <row r="256">
@@ -6784,10 +6784,10 @@
         <v>5894.0</v>
       </c>
       <c r="G256" t="n">
-        <v>3362.0</v>
+        <v>3517.0</v>
       </c>
       <c r="H256" t="n">
-        <v>0.04524479188352578</v>
+        <v>0.03257012884495354</v>
       </c>
     </row>
     <row r="257">
@@ -6810,10 +6810,10 @@
         <v>5894.0</v>
       </c>
       <c r="G257" t="n">
-        <v>2189.0</v>
+        <v>2357.0</v>
       </c>
       <c r="H257" t="n">
-        <v>0.01989313649361177</v>
+        <v>0.015136305845627345</v>
       </c>
     </row>
     <row r="258">
@@ -6836,10 +6836,10 @@
         <v>5894.0</v>
       </c>
       <c r="G258" t="n">
-        <v>2189.0</v>
+        <v>2357.0</v>
       </c>
       <c r="H258" t="n">
-        <v>0.03978627298722354</v>
+        <v>0.03027261169125469</v>
       </c>
     </row>
     <row r="259">
@@ -6862,10 +6862,10 @@
         <v>5894.0</v>
       </c>
       <c r="G259" t="n">
-        <v>2189.0</v>
+        <v>2357.0</v>
       </c>
       <c r="H259" t="n">
-        <v>0.07957254597444707</v>
+        <v>0.06054522338250938</v>
       </c>
     </row>
     <row r="260">
@@ -6888,10 +6888,10 @@
         <v>5894.0</v>
       </c>
       <c r="G260" t="n">
-        <v>1326.0</v>
+        <v>1492.0</v>
       </c>
       <c r="H260" t="n">
-        <v>0.038591610822190016</v>
+        <v>0.02954830375047737</v>
       </c>
     </row>
     <row r="261">
@@ -6914,10 +6914,10 @@
         <v>5894.0</v>
       </c>
       <c r="G261" t="n">
-        <v>1326.0</v>
+        <v>1492.0</v>
       </c>
       <c r="H261" t="n">
-        <v>0.07718322164438003</v>
+        <v>0.05909660750095474</v>
       </c>
     </row>
     <row r="262">
@@ -6940,10 +6940,10 @@
         <v>5894.0</v>
       </c>
       <c r="G262" t="n">
-        <v>1326.0</v>
+        <v>1492.0</v>
       </c>
       <c r="H262" t="n">
-        <v>0.15436644328876006</v>
+        <v>0.11819321500190948</v>
       </c>
     </row>
     <row r="263">
@@ -6966,10 +6966,10 @@
         <v>5894.0</v>
       </c>
       <c r="G263" t="n">
-        <v>779.0</v>
+        <v>920.0</v>
       </c>
       <c r="H263" t="n">
-        <v>0.07119348229777062</v>
+        <v>0.05589297240975632</v>
       </c>
     </row>
     <row r="264">
@@ -6992,10 +6992,10 @@
         <v>5894.0</v>
       </c>
       <c r="G264" t="n">
-        <v>779.0</v>
+        <v>920.0</v>
       </c>
       <c r="H264" t="n">
-        <v>0.14238696459554123</v>
+        <v>0.11178594481951264</v>
       </c>
     </row>
     <row r="265">
@@ -7018,10 +7018,10 @@
         <v>5894.0</v>
       </c>
       <c r="G265" t="n">
-        <v>779.0</v>
+        <v>920.0</v>
       </c>
       <c r="H265" t="n">
-        <v>0.28477392919108246</v>
+        <v>0.22357188963902527</v>
       </c>
     </row>
     <row r="266">
@@ -7044,10 +7044,10 @@
         <v>37.0</v>
       </c>
       <c r="G266" t="n">
-        <v>21.0</v>
+        <v>24.0</v>
       </c>
       <c r="H266" t="n">
-        <v>-0.009878134015259601</v>
+        <v>-0.012860747149689161</v>
       </c>
     </row>
     <row r="267">
@@ -7070,10 +7070,10 @@
         <v>37.0</v>
       </c>
       <c r="G267" t="n">
-        <v>21.0</v>
+        <v>24.0</v>
       </c>
       <c r="H267" t="n">
-        <v>-0.019756268030519202</v>
+        <v>-0.025721494299378322</v>
       </c>
     </row>
     <row r="268">
@@ -7096,10 +7096,10 @@
         <v>37.0</v>
       </c>
       <c r="G268" t="n">
-        <v>21.0</v>
+        <v>24.0</v>
       </c>
       <c r="H268" t="n">
-        <v>-0.039512536061038404</v>
+        <v>-0.051442988598756643</v>
       </c>
     </row>
     <row r="269">
@@ -7122,10 +7122,10 @@
         <v>37.0</v>
       </c>
       <c r="G269" t="n">
-        <v>17.0</v>
+        <v>19.0</v>
       </c>
       <c r="H269" t="n">
-        <v>-0.007440582823825151</v>
+        <v>-0.014474951449477622</v>
       </c>
     </row>
     <row r="270">
@@ -7148,10 +7148,10 @@
         <v>37.0</v>
       </c>
       <c r="G270" t="n">
-        <v>17.0</v>
+        <v>19.0</v>
       </c>
       <c r="H270" t="n">
-        <v>-0.014881165647650301</v>
+        <v>-0.028949902898955243</v>
       </c>
     </row>
     <row r="271">
@@ -7174,10 +7174,10 @@
         <v>37.0</v>
       </c>
       <c r="G271" t="n">
-        <v>17.0</v>
+        <v>19.0</v>
       </c>
       <c r="H271" t="n">
-        <v>-0.029762331295300603</v>
+        <v>-0.057899805797910486</v>
       </c>
     </row>
     <row r="272">
@@ -7203,7 +7203,7 @@
         <v>14.0</v>
       </c>
       <c r="H272" t="n">
-        <v>-0.009036089031907946</v>
+        <v>-0.009565693984065909</v>
       </c>
     </row>
     <row r="273">
@@ -7229,7 +7229,7 @@
         <v>14.0</v>
       </c>
       <c r="H273" t="n">
-        <v>-0.01807217806381589</v>
+        <v>-0.019131387968131817</v>
       </c>
     </row>
     <row r="274">
@@ -7255,7 +7255,7 @@
         <v>14.0</v>
       </c>
       <c r="H274" t="n">
-        <v>-0.03614435612763178</v>
+        <v>-0.038262775936263635</v>
       </c>
     </row>
     <row r="275">
@@ -7281,7 +7281,7 @@
         <v>6.0</v>
       </c>
       <c r="H275" t="n">
-        <v>0.013329612762394992</v>
+        <v>0.011639992939493651</v>
       </c>
     </row>
     <row r="276">
@@ -7307,7 +7307,7 @@
         <v>6.0</v>
       </c>
       <c r="H276" t="n">
-        <v>0.026659225524789984</v>
+        <v>0.023279985878987303</v>
       </c>
     </row>
     <row r="277">
@@ -7333,7 +7333,7 @@
         <v>6.0</v>
       </c>
       <c r="H277" t="n">
-        <v>0.05331845104957997</v>
+        <v>0.046559971757974605</v>
       </c>
     </row>
     <row r="278">
@@ -7356,10 +7356,10 @@
         <v>37.0</v>
       </c>
       <c r="G278" t="n">
-        <v>21.0</v>
+        <v>25.0</v>
       </c>
       <c r="H278" t="n">
-        <v>-0.010267586859708326</v>
+        <v>-0.013228729039230034</v>
       </c>
     </row>
     <row r="279">
@@ -7382,10 +7382,10 @@
         <v>37.0</v>
       </c>
       <c r="G279" t="n">
-        <v>21.0</v>
+        <v>25.0</v>
       </c>
       <c r="H279" t="n">
-        <v>-0.02053517371941665</v>
+        <v>-0.026457458078460068</v>
       </c>
     </row>
     <row r="280">
@@ -7408,10 +7408,10 @@
         <v>37.0</v>
       </c>
       <c r="G280" t="n">
-        <v>21.0</v>
+        <v>25.0</v>
       </c>
       <c r="H280" t="n">
-        <v>-0.0410703474388333</v>
+        <v>-0.052914916156920136</v>
       </c>
     </row>
     <row r="281">
@@ -7434,10 +7434,10 @@
         <v>37.0</v>
       </c>
       <c r="G281" t="n">
-        <v>17.0</v>
+        <v>19.0</v>
       </c>
       <c r="H281" t="n">
-        <v>-0.007814444316560004</v>
+        <v>-0.01489997528649194</v>
       </c>
     </row>
     <row r="282">
@@ -7460,10 +7460,10 @@
         <v>37.0</v>
       </c>
       <c r="G282" t="n">
-        <v>17.0</v>
+        <v>19.0</v>
       </c>
       <c r="H282" t="n">
-        <v>-0.01562888863312001</v>
+        <v>-0.02979995057298388</v>
       </c>
     </row>
     <row r="283">
@@ -7486,10 +7486,10 @@
         <v>37.0</v>
       </c>
       <c r="G283" t="n">
-        <v>17.0</v>
+        <v>19.0</v>
       </c>
       <c r="H283" t="n">
-        <v>-0.03125777726624002</v>
+        <v>-0.05959990114596776</v>
       </c>
     </row>
     <row r="284">
@@ -7515,7 +7515,7 @@
         <v>14.0</v>
       </c>
       <c r="H284" t="n">
-        <v>-0.00947524989110345</v>
+        <v>-0.009852302152832365</v>
       </c>
     </row>
     <row r="285">
@@ -7541,7 +7541,7 @@
         <v>14.0</v>
       </c>
       <c r="H285" t="n">
-        <v>-0.0189504997822069</v>
+        <v>-0.01970460430566473</v>
       </c>
     </row>
     <row r="286">
@@ -7567,7 +7567,7 @@
         <v>14.0</v>
       </c>
       <c r="H286" t="n">
-        <v>-0.0379009995644138</v>
+        <v>-0.03940920861132946</v>
       </c>
     </row>
     <row r="287">
@@ -7590,10 +7590,10 @@
         <v>37.0</v>
       </c>
       <c r="G287" t="n">
-        <v>6.0</v>
+        <v>5.0</v>
       </c>
       <c r="H287" t="n">
-        <v>0.013388504189123488</v>
+        <v>0.02471533791033746</v>
       </c>
     </row>
     <row r="288">
@@ -7616,10 +7616,10 @@
         <v>37.0</v>
       </c>
       <c r="G288" t="n">
-        <v>6.0</v>
+        <v>5.0</v>
       </c>
       <c r="H288" t="n">
-        <v>0.026777008378246977</v>
+        <v>0.04943067582067492</v>
       </c>
     </row>
     <row r="289">
@@ -7642,10 +7642,10 @@
         <v>37.0</v>
       </c>
       <c r="G289" t="n">
-        <v>6.0</v>
+        <v>5.0</v>
       </c>
       <c r="H289" t="n">
-        <v>0.053554016756493954</v>
+        <v>0.09886135164134983</v>
       </c>
     </row>
   </sheetData>

</xml_diff>